<commit_message>
Updated Instruction Set Again to include Parity Check
</commit_message>
<xml_diff>
--- a/architektur/InstructionSetV1.xlsx
+++ b/architektur/InstructionSetV1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPGA_CPU\architektur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E73BC97-EB29-4476-8BC0-9E3B730E32DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A45865-2116-4F5E-8D48-5EC6B8A48EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{C9158578-7B59-404A-A949-5211959D3F7E}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>ADD</t>
   </si>
@@ -139,6 +138,9 @@
   </si>
   <si>
     <t>WRMr</t>
+  </si>
+  <si>
+    <t>PAR</t>
   </si>
 </sst>
 </file>
@@ -525,7 +527,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="117" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -661,8 +663,14 @@
       <c r="B27" t="s">
         <v>0</v>
       </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
       <c r="D27" t="s">
         <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -670,10 +678,7 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated Instruction Set Again to remove Parity Check
</commit_message>
<xml_diff>
--- a/architektur/InstructionSetV1.xlsx
+++ b/architektur/InstructionSetV1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPGA_CPU\architektur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A45865-2116-4F5E-8D48-5EC6B8A48EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDC8431-D420-450B-82A4-BF96BE49F485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{C9158578-7B59-404A-A949-5211959D3F7E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>ADD</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>WRMr</t>
-  </si>
-  <si>
-    <t>PAR</t>
   </si>
 </sst>
 </file>
@@ -527,7 +524,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="117" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -677,9 +674,6 @@
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B28" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">

</xml_diff>

<commit_message>
Finished first functioning Architecture Prototype and ran first program
</commit_message>
<xml_diff>
--- a/architektur/InstructionSetV1.xlsx
+++ b/architektur/InstructionSetV1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPGA_CPU\architektur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDC8431-D420-450B-82A4-BF96BE49F485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DA6A7C-EE48-41F8-BBE3-25919A81C027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{C9158578-7B59-404A-A949-5211959D3F7E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>ADD</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>WRMr</t>
+  </si>
+  <si>
+    <t>EXT</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="117" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -625,6 +628,9 @@
       <c r="D22" t="s">
         <v>29</v>
       </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">

</xml_diff>

<commit_message>
Added CR and unified condintional branches
</commit_message>
<xml_diff>
--- a/architektur/InstructionSetV1.xlsx
+++ b/architektur/InstructionSetV1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPGA_CPU\architektur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B5089C-A2C9-4065-84AC-7FA5CCC9E986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8517DFE9-FA15-46AA-B60E-04E55876D52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{C9158578-7B59-404A-A949-5211959D3F7E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C9158578-7B59-404A-A949-5211959D3F7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>ADD</t>
   </si>
@@ -132,24 +132,6 @@
   </si>
   <si>
     <t>EXT</t>
-  </si>
-  <si>
-    <t>Pipeline</t>
-  </si>
-  <si>
-    <t>RF Read</t>
-  </si>
-  <si>
-    <t>RF Write</t>
-  </si>
-  <si>
-    <t>RAM Read</t>
-  </si>
-  <si>
-    <t>RAM Write</t>
-  </si>
-  <si>
-    <t>PC Write</t>
   </si>
 </sst>
 </file>
@@ -533,175 +515,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4F1C2-56A9-491C-9DAF-F70BC798C44A}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="117" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J7" t="s">
-        <v>5</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J8" t="s">
-        <v>29</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J10" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="O10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J12" t="s">
-        <v>15</v>
-      </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J14" t="s">
-        <v>31</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -709,7 +541,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -723,7 +555,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -740,7 +572,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -757,7 +589,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -771,7 +603,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
@@ -782,12 +614,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -795,7 +627,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
         <v>8</v>
       </c>
@@ -809,7 +641,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -826,12 +658,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
@@ -848,7 +680,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Removed IMH from Specs temporarily and implemented a big chunk of the Pipeline
</commit_message>
<xml_diff>
--- a/architektur/InstructionSetV1.xlsx
+++ b/architektur/InstructionSetV1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPGA_CPU\architektur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8517DFE9-FA15-46AA-B60E-04E55876D52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B5089C-A2C9-4065-84AC-7FA5CCC9E986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C9158578-7B59-404A-A949-5211959D3F7E}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{C9158578-7B59-404A-A949-5211959D3F7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>ADD</t>
   </si>
@@ -132,6 +132,24 @@
   </si>
   <si>
     <t>EXT</t>
+  </si>
+  <si>
+    <t>Pipeline</t>
+  </si>
+  <si>
+    <t>RF Read</t>
+  </si>
+  <si>
+    <t>RF Write</t>
+  </si>
+  <si>
+    <t>RAM Read</t>
+  </si>
+  <si>
+    <t>RAM Write</t>
+  </si>
+  <si>
+    <t>PC Write</t>
   </si>
 </sst>
 </file>
@@ -515,25 +533,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4F1C2-56A9-491C-9DAF-F70BC798C44A}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="117" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -541,7 +709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -555,7 +723,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -572,7 +740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -589,7 +757,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -603,7 +771,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
@@ -614,12 +782,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -627,7 +795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>8</v>
       </c>
@@ -641,7 +809,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -658,12 +826,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
@@ -680,7 +848,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>